<commit_message>
adatbazis terv kicsit csinositva
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Admin</t>
   </si>
@@ -35,86 +35,155 @@
     <t>Munkavállaló</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>emal</t>
-  </si>
-  <si>
-    <t>eletkor</t>
-  </si>
-  <si>
-    <t>felhasznalonev</t>
-  </si>
-  <si>
-    <t>felhasznalt_szabadsag</t>
-  </si>
-  <si>
-    <t>betegszabadsag</t>
-  </si>
-  <si>
-    <t>csusztatas</t>
-  </si>
-  <si>
-    <t>szabadsag_igenyles</t>
-  </si>
-  <si>
-    <t>szaadsag_elfogadas</t>
-  </si>
-  <si>
-    <t>munkavallalo_listazasa</t>
-  </si>
-  <si>
-    <t>munkavallalo_hozzaadasa</t>
-  </si>
-  <si>
     <t>cím</t>
   </si>
   <si>
-    <t>szabadsag_mennyisege</t>
-  </si>
-  <si>
-    <t>csaladi_allapot</t>
-  </si>
-  <si>
-    <t>fonok</t>
-  </si>
-  <si>
-    <t>fnev</t>
-  </si>
-  <si>
-    <t>munkavallalo_torlese</t>
-  </si>
-  <si>
-    <t>fonok_regisztralasa_elfogadasa</t>
-  </si>
-  <si>
-    <t>regisztracio</t>
-  </si>
-  <si>
-    <t>admin_hozzaadasa</t>
-  </si>
-  <si>
-    <t>fonok_torlese-&gt; hozza tartozo mv is</t>
-  </si>
-  <si>
-    <t>telephely_nev</t>
-  </si>
-  <si>
-    <t>reszleg_nev</t>
-  </si>
-  <si>
-    <t>beosztas</t>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>tagid</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>adid</t>
+  </si>
+  <si>
+    <t>fonid</t>
+  </si>
+  <si>
+    <t>munkid</t>
+  </si>
+  <si>
+    <t>alapbér</t>
+  </si>
+  <si>
+    <t>+ szabadsag_igenyles</t>
+  </si>
+  <si>
+    <t>+szabadsag_mennyisege</t>
+  </si>
+  <si>
+    <t>Munkahely</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>név</t>
+  </si>
+  <si>
+    <t>részleg</t>
+  </si>
+  <si>
+    <t>+ fonok_regisztralasa: Boolean</t>
+  </si>
+  <si>
+    <t>+ admin_hozzaadasa: Boolean</t>
+  </si>
+  <si>
+    <t>+ fonok_torlese</t>
+  </si>
+  <si>
+    <t>SzabadságMennyisége</t>
+  </si>
+  <si>
+    <t>szid</t>
+  </si>
+  <si>
+    <t>jelszó</t>
+  </si>
+  <si>
+    <t>életkor</t>
+  </si>
+  <si>
+    <t>Értesítések</t>
+  </si>
+  <si>
+    <t>eid</t>
+  </si>
+  <si>
+    <t>elfogadott</t>
+  </si>
+  <si>
+    <t>+ szabadsag_bevitele</t>
+  </si>
+  <si>
+    <t>+szabadság_elfogadása</t>
+  </si>
+  <si>
+    <t>+értesítések_lekérdezése</t>
+  </si>
+  <si>
+    <t>felhasználói_szint</t>
+  </si>
+  <si>
+    <t>felhasznált_szabadság</t>
+  </si>
+  <si>
+    <t>betegszabadság</t>
+  </si>
+  <si>
+    <t>csúsztatás</t>
+  </si>
+  <si>
+    <t>családi állapot</t>
+  </si>
+  <si>
+    <t>szöveg</t>
+  </si>
+  <si>
+    <t>munkavégzés_kezdete</t>
+  </si>
+  <si>
+    <t>fid</t>
+  </si>
+  <si>
+    <t>tárgyhó</t>
+  </si>
+  <si>
+    <t>fizetés</t>
+  </si>
+  <si>
+    <t>Fnév</t>
+  </si>
+  <si>
+    <t>+ szabadsag_elfogadas: Boolean</t>
+  </si>
+  <si>
+    <t>+ munkavallalok_listazasa: Array</t>
+  </si>
+  <si>
+    <t>+ munkavallalo_hozzaadasa</t>
+  </si>
+  <si>
+    <t>+ munkavallalo_torlese</t>
+  </si>
+  <si>
+    <t>+ szabadsag_mennyisege: Int</t>
+  </si>
+  <si>
+    <t>nid</t>
+  </si>
+  <si>
+    <t>MunkaÓra</t>
+  </si>
+  <si>
+    <t>KorábbiFizetések</t>
+  </si>
+  <si>
+    <t>nap</t>
+  </si>
+  <si>
+    <t>ledolgozott_perc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +200,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +226,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -154,19 +283,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+      <color rgb="FF66FFCC"/>
+      <color rgb="FFCC66FF"/>
+      <color rgb="FF9900FF"/>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -441,172 +679,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="C13" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="G22" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>